<commit_message>
Manual Watering South fixes and refactoring
</commit_message>
<xml_diff>
--- a/Documents/Implementation.xlsx
+++ b/Documents/Implementation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Androvil\Visual Studio 2013\Projects\HomeAutomation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5115FB07-10EC-45D0-8C3D-FF4D93A5ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E43D59-3CF0-4D1A-99C5-F3B570B17A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-480" windowWidth="29040" windowHeight="15525" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15075" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Custom Chars" sheetId="4" r:id="rId3"/>
     <sheet name="Expander" sheetId="3" r:id="rId4"/>
     <sheet name="LED" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
   <si>
     <t>:</t>
   </si>
@@ -359,15 +360,45 @@
   <si>
     <t>https://tashev-galving.com/cat/200383/kabeli-i-provodnitsi?filter.115.%D0%A1%D0%B5%D1%87%D0%B5%D0%BD%D0%B8%D0%B5+%D0%BD%D0%B0+%D0%BF%D1%80%D0%BE%D0%B2%D0%BE%D0%B4%D0%BD%D0%B8%D0%BA=1.5&amp;filter.73.%D0%91%D1%80%D0%BE%D0%B9+%D0%B6%D0%B8%D0%BB%D0%B0=4&amp;search=%D1%81%D0%B2%D1%82D0%BE%D0%B9+%D0%B6%D0%B8%D0%BB%D0%B0=3&amp;search=%D1%81%D0%B2%D1%82</t>
   </si>
+  <si>
+    <t>Time set</t>
+  </si>
+  <si>
+    <t>Bytes avilable</t>
+  </si>
+  <si>
+    <t>HardwareManager</t>
+  </si>
+  <si>
+    <t>SetupToolsAndServices</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>ReloadConfig</t>
+  </si>
+  <si>
+    <t>_autoTurnOffPumpService.Init()</t>
+  </si>
+  <si>
+    <t>UiManager</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -415,8 +446,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +470,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -613,11 +656,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +766,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -737,11 +783,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="15" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -803,7 +854,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F1020FB-56EC-C3E5-FEB3-0892EE40FC58}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -824,23 +875,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -868,7 +906,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1741AA3-6A8E-1AC7-28AB-853B97F440E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1111,7 +1149,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11A2A66A-895E-06C6-B48A-BA5ABB0EAA3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1439,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:Y31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1922,7 +1960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>22</v>
       </c>
@@ -1938,19 +1976,19 @@
       <c r="F17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="53">
         <v>2</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="53">
         <v>3</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="53">
         <v>4</v>
       </c>
-      <c r="K17" s="7"/>
+      <c r="K17" s="53"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
@@ -1974,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>23</v>
       </c>
@@ -1990,18 +2028,19 @@
       <c r="F18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="G18" s="54">
+        <v>1</v>
+      </c>
+      <c r="H18" s="54">
+        <v>0</v>
+      </c>
+      <c r="I18" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="54">
         <v>2</v>
       </c>
+      <c r="K18" s="54"/>
       <c r="S18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2021,7 +2060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>29</v>
       </c>
@@ -2037,15 +2076,17 @@
       <c r="F19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="G19" s="54">
+        <v>1</v>
+      </c>
+      <c r="H19" s="54">
         <v>2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="54">
         <v>3</v>
       </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
       <c r="L19" s="1" t="s">
         <v>30</v>
       </c>
@@ -2055,15 +2096,16 @@
       <c r="N19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O19" s="1">
-        <v>1</v>
-      </c>
-      <c r="P19" s="1">
+      <c r="O19" s="54">
+        <v>1</v>
+      </c>
+      <c r="P19" s="54">
         <v>2</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="54">
         <v>3</v>
       </c>
+      <c r="R19" s="54"/>
       <c r="S19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2550,11 +2592,11 @@
       <c r="I12">
         <v>0.09</v>
       </c>
-      <c r="L12" s="51">
+      <c r="L12" s="46">
         <f>(N12+O12)*M12/O12</f>
         <v>4.95</v>
       </c>
-      <c r="M12" s="52">
+      <c r="M12" s="47">
         <v>3.3</v>
       </c>
       <c r="N12">
@@ -2577,10 +2619,10 @@
       <c r="I13">
         <v>0.03</v>
       </c>
-      <c r="L13" s="52">
+      <c r="L13" s="47">
         <v>5</v>
       </c>
-      <c r="M13" s="51">
+      <c r="M13" s="46">
         <f>O13*L13/(O13+N13)</f>
         <v>3.3333333333333335</v>
       </c>
@@ -2604,10 +2646,10 @@
       <c r="I14">
         <v>0.04</v>
       </c>
-      <c r="L14" s="52">
+      <c r="L14" s="47">
         <v>5</v>
       </c>
-      <c r="M14" s="52">
+      <c r="M14" s="47">
         <v>3.3</v>
       </c>
       <c r="N14" s="41">
@@ -2631,10 +2673,10 @@
       <c r="I15">
         <v>0.06</v>
       </c>
-      <c r="L15" s="52">
+      <c r="L15" s="47">
         <v>5</v>
       </c>
-      <c r="M15" s="52">
+      <c r="M15" s="47">
         <v>3.3</v>
       </c>
       <c r="N15">
@@ -2798,7 +2840,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46">
+      <c r="A2" s="48">
         <v>0</v>
       </c>
       <c r="B2" s="36">
@@ -2816,7 +2858,7 @@
         <f>BIN2DEC(L2)</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="46">
+      <c r="Q2" s="48">
         <v>0</v>
       </c>
       <c r="R2" s="36">
@@ -2850,7 +2892,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="36">
         <v>1</v>
       </c>
@@ -2869,7 +2911,7 @@
         <f t="shared" ref="M3:M65" si="2">BIN2DEC(L3)</f>
         <v>4</v>
       </c>
-      <c r="Q3" s="47"/>
+      <c r="Q3" s="49"/>
       <c r="R3" s="36">
         <v>1</v>
       </c>
@@ -2900,7 +2942,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="36">
         <v>2</v>
       </c>
@@ -2922,7 +2964,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q4" s="47"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="36">
         <v>2</v>
       </c>
@@ -2950,7 +2992,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="36">
         <v>3</v>
       </c>
@@ -2969,7 +3011,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q5" s="47"/>
+      <c r="Q5" s="49"/>
       <c r="R5" s="36">
         <v>3</v>
       </c>
@@ -3000,7 +3042,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="36">
         <v>4</v>
       </c>
@@ -3019,7 +3061,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q6" s="47"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="36">
         <v>4</v>
       </c>
@@ -3047,7 +3089,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="36">
         <v>5</v>
       </c>
@@ -3066,7 +3108,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q7" s="47"/>
+      <c r="Q7" s="49"/>
       <c r="R7" s="36">
         <v>5</v>
       </c>
@@ -3094,7 +3136,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="36">
         <v>6</v>
       </c>
@@ -3119,7 +3161,7 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="Q8" s="47"/>
+      <c r="Q8" s="49"/>
       <c r="R8" s="36">
         <v>6</v>
       </c>
@@ -3153,7 +3195,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="37">
         <v>7</v>
       </c>
@@ -3177,7 +3219,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="48"/>
+      <c r="Q9" s="50"/>
       <c r="R9" s="37">
         <v>7</v>
       </c>
@@ -3220,7 +3262,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
+      <c r="A10" s="48">
         <v>1</v>
       </c>
       <c r="B10" s="36">
@@ -3238,7 +3280,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="48">
         <v>1</v>
       </c>
       <c r="R10" s="36">
@@ -3271,7 +3313,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="36">
         <v>1</v>
       </c>
@@ -3293,7 +3335,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q11" s="47"/>
+      <c r="Q11" s="49"/>
       <c r="R11" s="36">
         <v>1</v>
       </c>
@@ -3317,7 +3359,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="36">
         <v>2</v>
       </c>
@@ -3339,7 +3381,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q12" s="47"/>
+      <c r="Q12" s="49"/>
       <c r="R12" s="36">
         <v>2</v>
       </c>
@@ -3360,7 +3402,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="36">
         <v>3</v>
       </c>
@@ -3379,7 +3421,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q13" s="47"/>
+      <c r="Q13" s="49"/>
       <c r="R13" s="36">
         <v>3</v>
       </c>
@@ -3400,7 +3442,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="36">
         <v>4</v>
       </c>
@@ -3419,7 +3461,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q14" s="47"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="36">
         <v>4</v>
       </c>
@@ -3440,7 +3482,7 @@
       </c>
     </row>
     <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="36">
         <v>5</v>
       </c>
@@ -3459,7 +3501,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q15" s="47"/>
+      <c r="Q15" s="49"/>
       <c r="R15" s="36">
         <v>5</v>
       </c>
@@ -3480,7 +3522,7 @@
       </c>
     </row>
     <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="36">
         <v>6</v>
       </c>
@@ -3508,7 +3550,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q16" s="47"/>
+      <c r="Q16" s="49"/>
       <c r="R16" s="36">
         <v>6</v>
       </c>
@@ -3541,7 +3583,7 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="37">
         <v>7</v>
       </c>
@@ -3565,7 +3607,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="48"/>
+      <c r="Q17" s="50"/>
       <c r="R17" s="37">
         <v>7</v>
       </c>
@@ -3601,7 +3643,7 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+      <c r="A18" s="48">
         <v>2</v>
       </c>
       <c r="B18" s="36">
@@ -3619,7 +3661,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="46">
+      <c r="Q18" s="48">
         <v>2</v>
       </c>
       <c r="R18" s="36">
@@ -3658,7 +3700,7 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="36">
         <v>1</v>
       </c>
@@ -3686,7 +3728,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q19" s="47"/>
+      <c r="Q19" s="49"/>
       <c r="R19" s="36">
         <v>1</v>
       </c>
@@ -3707,7 +3749,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="36">
         <v>2</v>
       </c>
@@ -3726,7 +3768,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q20" s="47"/>
+      <c r="Q20" s="49"/>
       <c r="R20" s="36">
         <v>2</v>
       </c>
@@ -3750,7 +3792,7 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="36">
         <v>3</v>
       </c>
@@ -3769,7 +3811,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q21" s="47"/>
+      <c r="Q21" s="49"/>
       <c r="R21" s="36">
         <v>3</v>
       </c>
@@ -3790,7 +3832,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="36">
         <v>4</v>
       </c>
@@ -3809,7 +3851,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q22" s="47"/>
+      <c r="Q22" s="49"/>
       <c r="R22" s="36">
         <v>4</v>
       </c>
@@ -3830,7 +3872,7 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="36">
         <v>5</v>
       </c>
@@ -3852,7 +3894,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q23" s="47"/>
+      <c r="Q23" s="49"/>
       <c r="R23" s="36">
         <v>5</v>
       </c>
@@ -3876,7 +3918,7 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="36">
         <v>6</v>
       </c>
@@ -3898,7 +3940,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q24" s="47"/>
+      <c r="Q24" s="49"/>
       <c r="R24" s="36">
         <v>6</v>
       </c>
@@ -3925,7 +3967,7 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="37">
         <v>7</v>
       </c>
@@ -3949,7 +3991,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="48"/>
+      <c r="Q25" s="50"/>
       <c r="R25" s="37">
         <v>7</v>
       </c>
@@ -3985,7 +4027,7 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
+      <c r="A26" s="48">
         <v>3</v>
       </c>
       <c r="B26" s="36">
@@ -4003,7 +4045,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="46">
+      <c r="Q26" s="48">
         <v>3</v>
       </c>
       <c r="R26" s="36">
@@ -4033,7 +4075,7 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="36">
         <v>1</v>
       </c>
@@ -4052,7 +4094,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q27" s="47"/>
+      <c r="Q27" s="49"/>
       <c r="R27" s="36">
         <v>1</v>
       </c>
@@ -4076,7 +4118,7 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="36">
         <v>2</v>
       </c>
@@ -4098,7 +4140,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q28" s="47"/>
+      <c r="Q28" s="49"/>
       <c r="R28" s="36">
         <v>2</v>
       </c>
@@ -4122,7 +4164,7 @@
       </c>
     </row>
     <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="36">
         <v>3</v>
       </c>
@@ -4144,7 +4186,7 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="Q29" s="47"/>
+      <c r="Q29" s="49"/>
       <c r="R29" s="36">
         <v>3</v>
       </c>
@@ -4168,7 +4210,7 @@
       </c>
     </row>
     <row r="30" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="36">
         <v>4</v>
       </c>
@@ -4196,7 +4238,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q30" s="47"/>
+      <c r="Q30" s="49"/>
       <c r="R30" s="36">
         <v>4</v>
       </c>
@@ -4229,7 +4271,7 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="36">
         <v>5</v>
       </c>
@@ -4248,7 +4290,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q31" s="47"/>
+      <c r="Q31" s="49"/>
       <c r="R31" s="36">
         <v>5</v>
       </c>
@@ -4269,7 +4311,7 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="36">
         <v>6</v>
       </c>
@@ -4288,7 +4330,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q32" s="47"/>
+      <c r="Q32" s="49"/>
       <c r="R32" s="36">
         <v>6</v>
       </c>
@@ -4309,7 +4351,7 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="37">
         <v>7</v>
       </c>
@@ -4333,7 +4375,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="48"/>
+      <c r="Q33" s="50"/>
       <c r="R33" s="37">
         <v>7</v>
       </c>
@@ -4369,7 +4411,7 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
+      <c r="A34" s="48">
         <v>4</v>
       </c>
       <c r="B34" s="36">
@@ -4387,7 +4429,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="46">
+      <c r="Q34" s="48">
         <v>4</v>
       </c>
       <c r="R34" s="36">
@@ -4426,7 +4468,7 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="36">
         <v>1</v>
       </c>
@@ -4454,7 +4496,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q35" s="47"/>
+      <c r="Q35" s="49"/>
       <c r="R35" s="36">
         <v>1</v>
       </c>
@@ -4475,7 +4517,7 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="36">
         <v>2</v>
       </c>
@@ -4494,7 +4536,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q36" s="47"/>
+      <c r="Q36" s="49"/>
       <c r="R36" s="36">
         <v>2</v>
       </c>
@@ -4524,7 +4566,7 @@
       </c>
     </row>
     <row r="37" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="36">
         <v>3</v>
       </c>
@@ -4549,7 +4591,7 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="Q37" s="47"/>
+      <c r="Q37" s="49"/>
       <c r="R37" s="36">
         <v>3</v>
       </c>
@@ -4570,7 +4612,7 @@
       </c>
     </row>
     <row r="38" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="36">
         <v>4</v>
       </c>
@@ -4589,7 +4631,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q38" s="47"/>
+      <c r="Q38" s="49"/>
       <c r="R38" s="36">
         <v>4</v>
       </c>
@@ -4613,7 +4655,7 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="36">
         <v>5</v>
       </c>
@@ -4635,7 +4677,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q39" s="47"/>
+      <c r="Q39" s="49"/>
       <c r="R39" s="36">
         <v>5</v>
       </c>
@@ -4659,7 +4701,7 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="36">
         <v>6</v>
       </c>
@@ -4681,7 +4723,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q40" s="47"/>
+      <c r="Q40" s="49"/>
       <c r="R40" s="36">
         <v>6</v>
       </c>
@@ -4708,7 +4750,7 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="37">
         <v>7</v>
       </c>
@@ -4732,7 +4774,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="48"/>
+      <c r="Q41" s="50"/>
       <c r="R41" s="37">
         <v>7</v>
       </c>
@@ -4768,7 +4810,7 @@
       </c>
     </row>
     <row r="42" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46">
+      <c r="A42" s="48">
         <v>5</v>
       </c>
       <c r="B42" s="36">
@@ -4786,7 +4828,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="46">
+      <c r="Q42" s="48">
         <v>5</v>
       </c>
       <c r="R42" s="36">
@@ -4816,7 +4858,7 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="36">
         <v>1</v>
       </c>
@@ -4838,7 +4880,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q43" s="47"/>
+      <c r="Q43" s="49"/>
       <c r="R43" s="36">
         <v>1</v>
       </c>
@@ -4859,7 +4901,7 @@
       </c>
     </row>
     <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="36">
         <v>2</v>
       </c>
@@ -4878,7 +4920,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q44" s="47"/>
+      <c r="Q44" s="49"/>
       <c r="R44" s="36">
         <v>2</v>
       </c>
@@ -4902,7 +4944,7 @@
       </c>
     </row>
     <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="36">
         <v>3</v>
       </c>
@@ -4927,7 +4969,7 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="Q45" s="47"/>
+      <c r="Q45" s="49"/>
       <c r="R45" s="36">
         <v>3</v>
       </c>
@@ -4957,7 +4999,7 @@
       </c>
     </row>
     <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="49"/>
       <c r="B46" s="36">
         <v>4</v>
       </c>
@@ -4979,7 +5021,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q46" s="47"/>
+      <c r="Q46" s="49"/>
       <c r="R46" s="36">
         <v>4</v>
       </c>
@@ -5003,7 +5045,7 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="36">
         <v>5</v>
       </c>
@@ -5025,7 +5067,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q47" s="47"/>
+      <c r="Q47" s="49"/>
       <c r="R47" s="36">
         <v>5</v>
       </c>
@@ -5049,7 +5091,7 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="36">
         <v>6</v>
       </c>
@@ -5071,7 +5113,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q48" s="47"/>
+      <c r="Q48" s="49"/>
       <c r="R48" s="36">
         <v>6</v>
       </c>
@@ -5098,7 +5140,7 @@
       </c>
     </row>
     <row r="49" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="48"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="37">
         <v>7</v>
       </c>
@@ -5122,7 +5164,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q49" s="48"/>
+      <c r="Q49" s="50"/>
       <c r="R49" s="37">
         <v>7</v>
       </c>
@@ -5158,7 +5200,7 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46">
+      <c r="A50" s="48">
         <v>6</v>
       </c>
       <c r="B50" s="36">
@@ -5176,7 +5218,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q50" s="46">
+      <c r="Q50" s="48">
         <v>6</v>
       </c>
       <c r="R50" s="36">
@@ -5215,7 +5257,7 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="36">
         <v>1</v>
       </c>
@@ -5243,7 +5285,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q51" s="47"/>
+      <c r="Q51" s="49"/>
       <c r="R51" s="36">
         <v>1</v>
       </c>
@@ -5267,7 +5309,7 @@
       </c>
     </row>
     <row r="52" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="49"/>
       <c r="B52" s="36">
         <v>2</v>
       </c>
@@ -5286,7 +5328,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q52" s="47"/>
+      <c r="Q52" s="49"/>
       <c r="R52" s="36">
         <v>2</v>
       </c>
@@ -5307,7 +5349,7 @@
       </c>
     </row>
     <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
+      <c r="A53" s="49"/>
       <c r="B53" s="36">
         <v>3</v>
       </c>
@@ -5326,7 +5368,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q53" s="47"/>
+      <c r="Q53" s="49"/>
       <c r="R53" s="36">
         <v>3</v>
       </c>
@@ -5350,7 +5392,7 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
+      <c r="A54" s="49"/>
       <c r="B54" s="36">
         <v>4</v>
       </c>
@@ -5369,7 +5411,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q54" s="47"/>
+      <c r="Q54" s="49"/>
       <c r="R54" s="36">
         <v>4</v>
       </c>
@@ -5390,7 +5432,7 @@
       </c>
     </row>
     <row r="55" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="49"/>
       <c r="B55" s="36">
         <v>5</v>
       </c>
@@ -5409,7 +5451,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q55" s="47"/>
+      <c r="Q55" s="49"/>
       <c r="R55" s="36">
         <v>5</v>
       </c>
@@ -5430,7 +5472,7 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
+      <c r="A56" s="49"/>
       <c r="B56" s="36">
         <v>6</v>
       </c>
@@ -5449,7 +5491,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q56" s="47"/>
+      <c r="Q56" s="49"/>
       <c r="R56" s="36">
         <v>6</v>
       </c>
@@ -5470,7 +5512,7 @@
       </c>
     </row>
     <row r="57" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="48"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="37">
         <v>7</v>
       </c>
@@ -5494,7 +5536,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q57" s="48"/>
+      <c r="Q57" s="50"/>
       <c r="R57" s="37">
         <v>7</v>
       </c>
@@ -5530,7 +5572,7 @@
       </c>
     </row>
     <row r="58" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46">
+      <c r="A58" s="48">
         <v>7</v>
       </c>
       <c r="B58" s="36">
@@ -5548,7 +5590,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q58" s="46">
+      <c r="Q58" s="48">
         <v>7</v>
       </c>
       <c r="R58" s="36">
@@ -5581,7 +5623,7 @@
       </c>
     </row>
     <row r="59" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
+      <c r="A59" s="49"/>
       <c r="B59" s="36">
         <v>1</v>
       </c>
@@ -5603,7 +5645,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q59" s="47"/>
+      <c r="Q59" s="49"/>
       <c r="R59" s="36">
         <v>1</v>
       </c>
@@ -5627,7 +5669,7 @@
       </c>
     </row>
     <row r="60" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="49"/>
       <c r="B60" s="36">
         <v>2</v>
       </c>
@@ -5649,7 +5691,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q60" s="47"/>
+      <c r="Q60" s="49"/>
       <c r="R60" s="36">
         <v>2</v>
       </c>
@@ -5676,7 +5718,7 @@
       </c>
     </row>
     <row r="61" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="36">
         <v>3</v>
       </c>
@@ -5698,7 +5740,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q61" s="47"/>
+      <c r="Q61" s="49"/>
       <c r="R61" s="36">
         <v>3</v>
       </c>
@@ -5725,7 +5767,7 @@
       </c>
     </row>
     <row r="62" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
+      <c r="A62" s="49"/>
       <c r="B62" s="36">
         <v>4</v>
       </c>
@@ -5747,7 +5789,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q62" s="47"/>
+      <c r="Q62" s="49"/>
       <c r="R62" s="36">
         <v>4</v>
       </c>
@@ -5774,7 +5816,7 @@
       </c>
     </row>
     <row r="63" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="36">
         <v>5</v>
       </c>
@@ -5796,7 +5838,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q63" s="47"/>
+      <c r="Q63" s="49"/>
       <c r="R63" s="36">
         <v>5</v>
       </c>
@@ -5820,7 +5862,7 @@
       </c>
     </row>
     <row r="64" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
+      <c r="A64" s="49"/>
       <c r="B64" s="36">
         <v>6</v>
       </c>
@@ -5842,7 +5884,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q64" s="47"/>
+      <c r="Q64" s="49"/>
       <c r="R64" s="36">
         <v>6</v>
       </c>
@@ -5869,7 +5911,7 @@
       </c>
     </row>
     <row r="65" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="48"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="37">
         <v>7</v>
       </c>
@@ -5893,7 +5935,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q65" s="48"/>
+      <c r="Q65" s="50"/>
       <c r="R65" s="37">
         <v>7</v>
       </c>
@@ -6191,7 +6233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B0B658-2EBB-4F68-A170-FD0A4D0F2FFC}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12:F15"/>
     </sheetView>
   </sheetViews>
@@ -6315,7 +6357,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="51" t="s">
         <v>67</v>
       </c>
       <c r="B6">
@@ -6338,7 +6380,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7">
         <v>1.2</v>
       </c>
@@ -6487,4 +6529,153 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C2ADA7-8737-4066-A051-DC50FE14AA88}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>36360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>32244</v>
+      </c>
+      <c r="C3">
+        <f>B2-B3</f>
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>30960</v>
+      </c>
+      <c r="C4">
+        <f>B3-B4</f>
+        <v>1284</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5">
+        <v>25488</v>
+      </c>
+      <c r="C5">
+        <f>B4-B5</f>
+        <v>5472</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6">
+        <v>26340</v>
+      </c>
+      <c r="C6">
+        <f>B5-B6</f>
+        <v>-852</v>
+      </c>
+      <c r="E6">
+        <v>24744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7">
+        <v>19092</v>
+      </c>
+      <c r="C7">
+        <f>B6-B7</f>
+        <v>7248</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>19668</v>
+      </c>
+      <c r="C8">
+        <f>B7-B8</f>
+        <v>-576</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>19896</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <f>E19*D19/1000/60</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>12.4</v>
+      </c>
+      <c r="F20">
+        <f>E20*F19</f>
+        <v>10.333333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cancel watering, overlapping and totally separate schedules implemented
</commit_message>
<xml_diff>
--- a/Documents/Implementation.xlsx
+++ b/Documents/Implementation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Androvil\Visual Studio 2013\Projects\HomeAutomation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E43D59-3CF0-4D1A-99C5-F3B570B17A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3277522-0FC9-4D91-AB9F-0FFB6A7929A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15075" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,11 +21,25 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="96">
   <si>
     <t>:</t>
   </si>
@@ -111,19 +125,10 @@
     <t>A</t>
   </si>
   <si>
-    <t>SD card status</t>
-  </si>
-  <si>
     <t>Water North/South (litres)</t>
   </si>
   <si>
     <t>W</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Pump status</t>
   </si>
   <si>
     <t>4х1.5</t>
@@ -389,6 +394,36 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>E/D</t>
+  </si>
+  <si>
+    <t>Relay Id</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -661,7 +696,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,6 +803,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,12 +830,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1475,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:Y31"/>
+  <dimension ref="A4:AV38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY24" sqref="AY24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1960,7 +2002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>22</v>
       </c>
@@ -1968,33 +2010,41 @@
         <v>0</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="53">
-        <v>2</v>
-      </c>
-      <c r="H17" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="53">
-        <v>3</v>
-      </c>
-      <c r="J17" s="53">
-        <v>4</v>
-      </c>
-      <c r="K17" s="53"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7">
         <v>0</v>
@@ -2012,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>23</v>
       </c>
@@ -2028,47 +2078,52 @@
       <c r="F18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="54">
-        <v>1</v>
-      </c>
-      <c r="H18" s="54">
-        <v>0</v>
-      </c>
-      <c r="I18" s="54" t="s">
+      <c r="G18" s="49">
+        <v>1</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0</v>
+      </c>
+      <c r="I18" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="49">
         <v>2</v>
       </c>
-      <c r="K18" s="54"/>
-      <c r="S18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y18" t="s">
+      <c r="K18" s="49"/>
+      <c r="L18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="49">
+        <v>2</v>
+      </c>
+      <c r="P18" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="49">
+        <v>3</v>
+      </c>
+      <c r="R18" s="49">
+        <v>4</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>29</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>25</v>
@@ -2076,19 +2131,19 @@
       <c r="F19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="54">
-        <v>1</v>
-      </c>
-      <c r="H19" s="54">
+      <c r="G19" s="49">
+        <v>1</v>
+      </c>
+      <c r="H19" s="49">
         <v>2</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I19" s="49">
         <v>3</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
       <c r="L19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>19</v>
@@ -2096,38 +2151,21 @@
       <c r="N19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O19" s="54">
-        <v>1</v>
-      </c>
-      <c r="P19" s="54">
+      <c r="O19" s="49">
+        <v>1</v>
+      </c>
+      <c r="P19" s="49">
         <v>2</v>
       </c>
-      <c r="Q19" s="54">
+      <c r="Q19" s="49">
         <v>3</v>
       </c>
-      <c r="R19" s="54"/>
-      <c r="S19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="R19" s="49"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C20" s="12">
         <v>3</v>
@@ -2145,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>0</v>
@@ -2170,7 +2208,7 @@
         <v>7</v>
       </c>
       <c r="Q20" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R20" s="14" t="s">
         <v>0</v>
@@ -2191,10 +2229,10 @@
         <v>4</v>
       </c>
       <c r="Y20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D24" s="2">
         <v>0</v>
       </c>
@@ -2256,7 +2294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
         <v>22</v>
       </c>
@@ -2264,30 +2302,38 @@
         <v>0</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="7">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="7">
-        <v>3</v>
-      </c>
-      <c r="J25" s="7">
-        <v>4</v>
-      </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
@@ -2307,8 +2353,19 @@
       <c r="W25" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="51"/>
+      <c r="AT25" s="51"/>
+      <c r="AU25" s="51"/>
+      <c r="AV25" s="51"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
         <v>23</v>
       </c>
@@ -2336,34 +2393,38 @@
       <c r="J26" s="1">
         <v>2</v>
       </c>
-      <c r="S26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W26" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y26" t="s">
+      <c r="L26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>2</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>3</v>
+      </c>
+      <c r="R26" s="1">
+        <v>4</v>
+      </c>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>29</v>
       </c>
       <c r="C27" s="9">
         <v>2</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>25</v>
@@ -2381,7 +2442,7 @@
         <v>3</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>19</v>
@@ -2398,28 +2459,11 @@
       <c r="Q27" s="1">
         <v>3</v>
       </c>
-      <c r="S27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C28" s="12">
         <v>3</v>
@@ -2428,7 +2472,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>0</v>
@@ -2459,7 +2503,7 @@
         <v>19</v>
       </c>
       <c r="P28" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q28" s="14" t="s">
         <v>0</v>
@@ -2481,14 +2525,287 @@
       </c>
       <c r="W28" s="15"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
       <c r="R30" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
       <c r="R31" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="G33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>2</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+      <c r="H34" s="3">
+        <v>4</v>
+      </c>
+      <c r="I34" s="3">
+        <v>5</v>
+      </c>
+      <c r="J34" s="3">
+        <v>6</v>
+      </c>
+      <c r="K34" s="3">
+        <v>7</v>
+      </c>
+      <c r="L34" s="3">
+        <v>8</v>
+      </c>
+      <c r="M34" s="3">
+        <v>9</v>
+      </c>
+      <c r="N34" s="3">
+        <v>10</v>
+      </c>
+      <c r="O34" s="3">
+        <v>11</v>
+      </c>
+      <c r="P34" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>13</v>
+      </c>
+      <c r="R34" s="3">
+        <v>14</v>
+      </c>
+      <c r="S34" s="3">
+        <v>15</v>
+      </c>
+      <c r="T34" s="3">
+        <v>16</v>
+      </c>
+      <c r="U34" s="3">
+        <v>17</v>
+      </c>
+      <c r="V34" s="3">
+        <v>18</v>
+      </c>
+      <c r="W34" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="7">
+        <v>1</v>
+      </c>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>2</v>
+      </c>
+      <c r="R35" s="7">
+        <v>2</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T35" s="7">
+        <v>0</v>
+      </c>
+      <c r="U35" s="7">
+        <v>0</v>
+      </c>
+      <c r="V35" s="7"/>
+      <c r="W35" s="8"/>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>6</v>
+      </c>
+      <c r="R36" s="1">
+        <v>5</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W36" s="11"/>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C37" s="9">
+        <v>2</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W37" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.2">
+      <c r="C38" s="12">
+        <v>3</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="O38" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="14">
+        <v>1</v>
+      </c>
+      <c r="R38" s="14">
+        <v>0</v>
+      </c>
+      <c r="S38" s="14">
+        <v>1</v>
+      </c>
+      <c r="T38" s="14">
+        <v>0</v>
+      </c>
+      <c r="U38" s="14">
+        <v>1</v>
+      </c>
+      <c r="V38" s="14">
+        <v>0</v>
+      </c>
+      <c r="W38" s="15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2523,10 +2840,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>2.2599999999999998</v>
@@ -2539,12 +2856,12 @@
         <v>225.99999999999997</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>35.07</v>
@@ -2557,29 +2874,29 @@
         <v>175.35</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="O11" s="22" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <f>SUM(B13:B23)</f>
@@ -2587,7 +2904,7 @@
       </c>
       <c r="D12" s="23"/>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I12">
         <v>0.09</v>
@@ -2608,13 +2925,13 @@
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I13">
         <v>0.03</v>
@@ -2635,13 +2952,13 @@
     </row>
     <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I14">
         <v>0.04</v>
@@ -2662,13 +2979,13 @@
     </row>
     <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I15">
         <v>0.06</v>
@@ -2689,7 +3006,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2698,7 +3015,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2706,7 +3023,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2840,7 +3157,7 @@
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
+      <c r="A2" s="53">
         <v>0</v>
       </c>
       <c r="B2" s="36">
@@ -2858,7 +3175,7 @@
         <f>BIN2DEC(L2)</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="48">
+      <c r="Q2" s="53">
         <v>0</v>
       </c>
       <c r="R2" s="36">
@@ -2892,7 +3209,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="36">
         <v>1</v>
       </c>
@@ -2911,7 +3228,7 @@
         <f t="shared" ref="M3:M65" si="2">BIN2DEC(L3)</f>
         <v>4</v>
       </c>
-      <c r="Q3" s="49"/>
+      <c r="Q3" s="54"/>
       <c r="R3" s="36">
         <v>1</v>
       </c>
@@ -2942,7 +3259,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="36">
         <v>2</v>
       </c>
@@ -2964,7 +3281,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q4" s="49"/>
+      <c r="Q4" s="54"/>
       <c r="R4" s="36">
         <v>2</v>
       </c>
@@ -2992,7 +3309,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="36">
         <v>3</v>
       </c>
@@ -3011,7 +3328,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q5" s="49"/>
+      <c r="Q5" s="54"/>
       <c r="R5" s="36">
         <v>3</v>
       </c>
@@ -3042,7 +3359,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="36">
         <v>4</v>
       </c>
@@ -3061,7 +3378,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q6" s="49"/>
+      <c r="Q6" s="54"/>
       <c r="R6" s="36">
         <v>4</v>
       </c>
@@ -3089,7 +3406,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="36">
         <v>5</v>
       </c>
@@ -3108,7 +3425,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q7" s="49"/>
+      <c r="Q7" s="54"/>
       <c r="R7" s="36">
         <v>5</v>
       </c>
@@ -3136,7 +3453,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="36">
         <v>6</v>
       </c>
@@ -3161,7 +3478,7 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="Q8" s="49"/>
+      <c r="Q8" s="54"/>
       <c r="R8" s="36">
         <v>6</v>
       </c>
@@ -3195,7 +3512,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="37">
         <v>7</v>
       </c>
@@ -3219,7 +3536,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="50"/>
+      <c r="Q9" s="55"/>
       <c r="R9" s="37">
         <v>7</v>
       </c>
@@ -3262,7 +3579,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48">
+      <c r="A10" s="53">
         <v>1</v>
       </c>
       <c r="B10" s="36">
@@ -3280,7 +3597,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="48">
+      <c r="Q10" s="53">
         <v>1</v>
       </c>
       <c r="R10" s="36">
@@ -3313,7 +3630,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="36">
         <v>1</v>
       </c>
@@ -3335,7 +3652,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q11" s="49"/>
+      <c r="Q11" s="54"/>
       <c r="R11" s="36">
         <v>1</v>
       </c>
@@ -3359,7 +3676,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="36">
         <v>2</v>
       </c>
@@ -3381,7 +3698,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q12" s="49"/>
+      <c r="Q12" s="54"/>
       <c r="R12" s="36">
         <v>2</v>
       </c>
@@ -3402,7 +3719,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="36">
         <v>3</v>
       </c>
@@ -3421,7 +3738,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q13" s="49"/>
+      <c r="Q13" s="54"/>
       <c r="R13" s="36">
         <v>3</v>
       </c>
@@ -3442,7 +3759,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="36">
         <v>4</v>
       </c>
@@ -3461,7 +3778,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q14" s="49"/>
+      <c r="Q14" s="54"/>
       <c r="R14" s="36">
         <v>4</v>
       </c>
@@ -3482,7 +3799,7 @@
       </c>
     </row>
     <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="36">
         <v>5</v>
       </c>
@@ -3501,7 +3818,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q15" s="49"/>
+      <c r="Q15" s="54"/>
       <c r="R15" s="36">
         <v>5</v>
       </c>
@@ -3522,7 +3839,7 @@
       </c>
     </row>
     <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="36">
         <v>6</v>
       </c>
@@ -3550,7 +3867,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q16" s="49"/>
+      <c r="Q16" s="54"/>
       <c r="R16" s="36">
         <v>6</v>
       </c>
@@ -3583,7 +3900,7 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="37">
         <v>7</v>
       </c>
@@ -3607,7 +3924,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="50"/>
+      <c r="Q17" s="55"/>
       <c r="R17" s="37">
         <v>7</v>
       </c>
@@ -3643,7 +3960,7 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48">
+      <c r="A18" s="53">
         <v>2</v>
       </c>
       <c r="B18" s="36">
@@ -3661,7 +3978,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="48">
+      <c r="Q18" s="53">
         <v>2</v>
       </c>
       <c r="R18" s="36">
@@ -3700,7 +4017,7 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="36">
         <v>1</v>
       </c>
@@ -3728,7 +4045,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q19" s="49"/>
+      <c r="Q19" s="54"/>
       <c r="R19" s="36">
         <v>1</v>
       </c>
@@ -3749,7 +4066,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="36">
         <v>2</v>
       </c>
@@ -3768,7 +4085,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q20" s="49"/>
+      <c r="Q20" s="54"/>
       <c r="R20" s="36">
         <v>2</v>
       </c>
@@ -3792,7 +4109,7 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="36">
         <v>3</v>
       </c>
@@ -3811,7 +4128,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q21" s="49"/>
+      <c r="Q21" s="54"/>
       <c r="R21" s="36">
         <v>3</v>
       </c>
@@ -3832,7 +4149,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="36">
         <v>4</v>
       </c>
@@ -3851,7 +4168,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q22" s="49"/>
+      <c r="Q22" s="54"/>
       <c r="R22" s="36">
         <v>4</v>
       </c>
@@ -3872,7 +4189,7 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="36">
         <v>5</v>
       </c>
@@ -3894,7 +4211,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q23" s="49"/>
+      <c r="Q23" s="54"/>
       <c r="R23" s="36">
         <v>5</v>
       </c>
@@ -3918,7 +4235,7 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="36">
         <v>6</v>
       </c>
@@ -3940,7 +4257,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q24" s="49"/>
+      <c r="Q24" s="54"/>
       <c r="R24" s="36">
         <v>6</v>
       </c>
@@ -3967,7 +4284,7 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="37">
         <v>7</v>
       </c>
@@ -3991,7 +4308,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="50"/>
+      <c r="Q25" s="55"/>
       <c r="R25" s="37">
         <v>7</v>
       </c>
@@ -4027,7 +4344,7 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48">
+      <c r="A26" s="53">
         <v>3</v>
       </c>
       <c r="B26" s="36">
@@ -4045,7 +4362,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="48">
+      <c r="Q26" s="53">
         <v>3</v>
       </c>
       <c r="R26" s="36">
@@ -4075,7 +4392,7 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="36">
         <v>1</v>
       </c>
@@ -4094,7 +4411,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q27" s="49"/>
+      <c r="Q27" s="54"/>
       <c r="R27" s="36">
         <v>1</v>
       </c>
@@ -4118,7 +4435,7 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="36">
         <v>2</v>
       </c>
@@ -4140,7 +4457,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q28" s="49"/>
+      <c r="Q28" s="54"/>
       <c r="R28" s="36">
         <v>2</v>
       </c>
@@ -4164,7 +4481,7 @@
       </c>
     </row>
     <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="36">
         <v>3</v>
       </c>
@@ -4186,7 +4503,7 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="Q29" s="49"/>
+      <c r="Q29" s="54"/>
       <c r="R29" s="36">
         <v>3</v>
       </c>
@@ -4210,7 +4527,7 @@
       </c>
     </row>
     <row r="30" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="36">
         <v>4</v>
       </c>
@@ -4238,7 +4555,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q30" s="49"/>
+      <c r="Q30" s="54"/>
       <c r="R30" s="36">
         <v>4</v>
       </c>
@@ -4271,7 +4588,7 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="36">
         <v>5</v>
       </c>
@@ -4290,7 +4607,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q31" s="49"/>
+      <c r="Q31" s="54"/>
       <c r="R31" s="36">
         <v>5</v>
       </c>
@@ -4311,7 +4628,7 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="36">
         <v>6</v>
       </c>
@@ -4330,7 +4647,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q32" s="49"/>
+      <c r="Q32" s="54"/>
       <c r="R32" s="36">
         <v>6</v>
       </c>
@@ -4351,7 +4668,7 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="37">
         <v>7</v>
       </c>
@@ -4375,7 +4692,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="50"/>
+      <c r="Q33" s="55"/>
       <c r="R33" s="37">
         <v>7</v>
       </c>
@@ -4411,7 +4728,7 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="48">
+      <c r="A34" s="53">
         <v>4</v>
       </c>
       <c r="B34" s="36">
@@ -4429,7 +4746,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="48">
+      <c r="Q34" s="53">
         <v>4</v>
       </c>
       <c r="R34" s="36">
@@ -4468,7 +4785,7 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="36">
         <v>1</v>
       </c>
@@ -4496,7 +4813,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q35" s="49"/>
+      <c r="Q35" s="54"/>
       <c r="R35" s="36">
         <v>1</v>
       </c>
@@ -4517,7 +4834,7 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="36">
         <v>2</v>
       </c>
@@ -4536,7 +4853,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q36" s="49"/>
+      <c r="Q36" s="54"/>
       <c r="R36" s="36">
         <v>2</v>
       </c>
@@ -4566,7 +4883,7 @@
       </c>
     </row>
     <row r="37" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
+      <c r="A37" s="54"/>
       <c r="B37" s="36">
         <v>3</v>
       </c>
@@ -4591,7 +4908,7 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="Q37" s="49"/>
+      <c r="Q37" s="54"/>
       <c r="R37" s="36">
         <v>3</v>
       </c>
@@ -4612,7 +4929,7 @@
       </c>
     </row>
     <row r="38" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
+      <c r="A38" s="54"/>
       <c r="B38" s="36">
         <v>4</v>
       </c>
@@ -4631,7 +4948,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q38" s="49"/>
+      <c r="Q38" s="54"/>
       <c r="R38" s="36">
         <v>4</v>
       </c>
@@ -4655,7 +4972,7 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="36">
         <v>5</v>
       </c>
@@ -4677,7 +4994,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q39" s="49"/>
+      <c r="Q39" s="54"/>
       <c r="R39" s="36">
         <v>5</v>
       </c>
@@ -4701,7 +5018,7 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="36">
         <v>6</v>
       </c>
@@ -4723,7 +5040,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q40" s="49"/>
+      <c r="Q40" s="54"/>
       <c r="R40" s="36">
         <v>6</v>
       </c>
@@ -4750,7 +5067,7 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="37">
         <v>7</v>
       </c>
@@ -4774,7 +5091,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="50"/>
+      <c r="Q41" s="55"/>
       <c r="R41" s="37">
         <v>7</v>
       </c>
@@ -4810,7 +5127,7 @@
       </c>
     </row>
     <row r="42" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="48">
+      <c r="A42" s="53">
         <v>5</v>
       </c>
       <c r="B42" s="36">
@@ -4828,7 +5145,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="48">
+      <c r="Q42" s="53">
         <v>5</v>
       </c>
       <c r="R42" s="36">
@@ -4858,7 +5175,7 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="36">
         <v>1</v>
       </c>
@@ -4880,7 +5197,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q43" s="49"/>
+      <c r="Q43" s="54"/>
       <c r="R43" s="36">
         <v>1</v>
       </c>
@@ -4901,7 +5218,7 @@
       </c>
     </row>
     <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
+      <c r="A44" s="54"/>
       <c r="B44" s="36">
         <v>2</v>
       </c>
@@ -4920,7 +5237,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q44" s="49"/>
+      <c r="Q44" s="54"/>
       <c r="R44" s="36">
         <v>2</v>
       </c>
@@ -4944,7 +5261,7 @@
       </c>
     </row>
     <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="36">
         <v>3</v>
       </c>
@@ -4969,7 +5286,7 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="Q45" s="49"/>
+      <c r="Q45" s="54"/>
       <c r="R45" s="36">
         <v>3</v>
       </c>
@@ -4999,7 +5316,7 @@
       </c>
     </row>
     <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
+      <c r="A46" s="54"/>
       <c r="B46" s="36">
         <v>4</v>
       </c>
@@ -5021,7 +5338,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q46" s="49"/>
+      <c r="Q46" s="54"/>
       <c r="R46" s="36">
         <v>4</v>
       </c>
@@ -5045,7 +5362,7 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
+      <c r="A47" s="54"/>
       <c r="B47" s="36">
         <v>5</v>
       </c>
@@ -5067,7 +5384,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q47" s="49"/>
+      <c r="Q47" s="54"/>
       <c r="R47" s="36">
         <v>5</v>
       </c>
@@ -5091,7 +5408,7 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
+      <c r="A48" s="54"/>
       <c r="B48" s="36">
         <v>6</v>
       </c>
@@ -5113,7 +5430,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q48" s="49"/>
+      <c r="Q48" s="54"/>
       <c r="R48" s="36">
         <v>6</v>
       </c>
@@ -5140,7 +5457,7 @@
       </c>
     </row>
     <row r="49" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
+      <c r="A49" s="55"/>
       <c r="B49" s="37">
         <v>7</v>
       </c>
@@ -5164,7 +5481,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q49" s="50"/>
+      <c r="Q49" s="55"/>
       <c r="R49" s="37">
         <v>7</v>
       </c>
@@ -5200,7 +5517,7 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="48">
+      <c r="A50" s="53">
         <v>6</v>
       </c>
       <c r="B50" s="36">
@@ -5218,7 +5535,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q50" s="48">
+      <c r="Q50" s="53">
         <v>6</v>
       </c>
       <c r="R50" s="36">
@@ -5257,7 +5574,7 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="36">
         <v>1</v>
       </c>
@@ -5285,7 +5602,7 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q51" s="49"/>
+      <c r="Q51" s="54"/>
       <c r="R51" s="36">
         <v>1</v>
       </c>
@@ -5309,7 +5626,7 @@
       </c>
     </row>
     <row r="52" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="36">
         <v>2</v>
       </c>
@@ -5328,7 +5645,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q52" s="49"/>
+      <c r="Q52" s="54"/>
       <c r="R52" s="36">
         <v>2</v>
       </c>
@@ -5349,7 +5666,7 @@
       </c>
     </row>
     <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="36">
         <v>3</v>
       </c>
@@ -5368,7 +5685,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q53" s="49"/>
+      <c r="Q53" s="54"/>
       <c r="R53" s="36">
         <v>3</v>
       </c>
@@ -5392,7 +5709,7 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
+      <c r="A54" s="54"/>
       <c r="B54" s="36">
         <v>4</v>
       </c>
@@ -5411,7 +5728,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q54" s="49"/>
+      <c r="Q54" s="54"/>
       <c r="R54" s="36">
         <v>4</v>
       </c>
@@ -5432,7 +5749,7 @@
       </c>
     </row>
     <row r="55" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="49"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="36">
         <v>5</v>
       </c>
@@ -5451,7 +5768,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q55" s="49"/>
+      <c r="Q55" s="54"/>
       <c r="R55" s="36">
         <v>5</v>
       </c>
@@ -5472,7 +5789,7 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
+      <c r="A56" s="54"/>
       <c r="B56" s="36">
         <v>6</v>
       </c>
@@ -5491,7 +5808,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q56" s="49"/>
+      <c r="Q56" s="54"/>
       <c r="R56" s="36">
         <v>6</v>
       </c>
@@ -5512,7 +5829,7 @@
       </c>
     </row>
     <row r="57" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
+      <c r="A57" s="55"/>
       <c r="B57" s="37">
         <v>7</v>
       </c>
@@ -5536,7 +5853,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q57" s="50"/>
+      <c r="Q57" s="55"/>
       <c r="R57" s="37">
         <v>7</v>
       </c>
@@ -5572,7 +5889,7 @@
       </c>
     </row>
     <row r="58" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="48">
+      <c r="A58" s="53">
         <v>7</v>
       </c>
       <c r="B58" s="36">
@@ -5590,7 +5907,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q58" s="48">
+      <c r="Q58" s="53">
         <v>7</v>
       </c>
       <c r="R58" s="36">
@@ -5623,7 +5940,7 @@
       </c>
     </row>
     <row r="59" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="49"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="36">
         <v>1</v>
       </c>
@@ -5645,7 +5962,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q59" s="49"/>
+      <c r="Q59" s="54"/>
       <c r="R59" s="36">
         <v>1</v>
       </c>
@@ -5669,7 +5986,7 @@
       </c>
     </row>
     <row r="60" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="49"/>
+      <c r="A60" s="54"/>
       <c r="B60" s="36">
         <v>2</v>
       </c>
@@ -5691,7 +6008,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q60" s="49"/>
+      <c r="Q60" s="54"/>
       <c r="R60" s="36">
         <v>2</v>
       </c>
@@ -5718,7 +6035,7 @@
       </c>
     </row>
     <row r="61" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49"/>
+      <c r="A61" s="54"/>
       <c r="B61" s="36">
         <v>3</v>
       </c>
@@ -5740,7 +6057,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q61" s="49"/>
+      <c r="Q61" s="54"/>
       <c r="R61" s="36">
         <v>3</v>
       </c>
@@ -5767,7 +6084,7 @@
       </c>
     </row>
     <row r="62" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49"/>
+      <c r="A62" s="54"/>
       <c r="B62" s="36">
         <v>4</v>
       </c>
@@ -5789,7 +6106,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q62" s="49"/>
+      <c r="Q62" s="54"/>
       <c r="R62" s="36">
         <v>4</v>
       </c>
@@ -5816,7 +6133,7 @@
       </c>
     </row>
     <row r="63" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49"/>
+      <c r="A63" s="54"/>
       <c r="B63" s="36">
         <v>5</v>
       </c>
@@ -5838,7 +6155,7 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q63" s="49"/>
+      <c r="Q63" s="54"/>
       <c r="R63" s="36">
         <v>5</v>
       </c>
@@ -5862,7 +6179,7 @@
       </c>
     </row>
     <row r="64" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49"/>
+      <c r="A64" s="54"/>
       <c r="B64" s="36">
         <v>6</v>
       </c>
@@ -5884,7 +6201,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q64" s="49"/>
+      <c r="Q64" s="54"/>
       <c r="R64" s="36">
         <v>6</v>
       </c>
@@ -5911,7 +6228,7 @@
       </c>
     </row>
     <row r="65" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="50"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="37">
         <v>7</v>
       </c>
@@ -5935,7 +6252,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q65" s="50"/>
+      <c r="Q65" s="55"/>
       <c r="R65" s="37">
         <v>7</v>
       </c>
@@ -6016,10 +6333,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -6052,7 +6369,7 @@
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -6095,7 +6412,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6249,47 +6566,47 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="43">
         <v>330</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E1" s="45">
         <v>5</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>3.16</v>
@@ -6312,7 +6629,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>2.0299999999999998</v>
@@ -6335,7 +6652,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>2.0699999999999998</v>
@@ -6357,8 +6674,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
-        <v>67</v>
+      <c r="A6" s="56" t="s">
+        <v>64</v>
       </c>
       <c r="B6">
         <v>2.2000000000000002</v>
@@ -6380,7 +6697,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+      <c r="A7" s="57"/>
       <c r="B7">
         <v>1.2</v>
       </c>
@@ -6402,7 +6719,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -6547,18 +6864,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>36360</v>
@@ -6566,25 +6883,25 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>32244</v>
       </c>
       <c r="C3">
-        <f>B2-B3</f>
+        <f t="shared" ref="C3:C8" si="0">B2-B3</f>
         <v>4116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4">
         <v>30960</v>
       </c>
       <c r="C4">
-        <f>B3-B4</f>
+        <f t="shared" si="0"/>
         <v>1284</v>
       </c>
       <c r="D4">
@@ -6593,13 +6910,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>25488</v>
       </c>
       <c r="C5">
-        <f>B4-B5</f>
+        <f t="shared" si="0"/>
         <v>5472</v>
       </c>
       <c r="D5">
@@ -6608,13 +6925,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>26340</v>
       </c>
       <c r="C6">
-        <f>B5-B6</f>
+        <f t="shared" si="0"/>
         <v>-852</v>
       </c>
       <c r="E6">
@@ -6623,13 +6940,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>19092</v>
       </c>
       <c r="C7">
-        <f>B6-B7</f>
+        <f t="shared" si="0"/>
         <v>7248</v>
       </c>
       <c r="D7">
@@ -6638,13 +6955,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>19668</v>
       </c>
       <c r="C8">
-        <f>B7-B8</f>
+        <f t="shared" si="0"/>
         <v>-576</v>
       </c>
       <c r="D8">

</xml_diff>